<commit_message>
Update data files: RMT-expense-analysis-chunk2.xlsx and expense-analysis.xlsx
</commit_message>
<xml_diff>
--- a/public/RMT-expense-analysis-chunk2.xlsx
+++ b/public/RMT-expense-analysis-chunk2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CDD565E-57E3-A54F-8280-FA5AA890F1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66095C93-7C91-8A4B-A4FA-2D32DCDCBCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="21200" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="105">
   <si>
     <t>Category</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>2025-05-01 00:00:00</t>
-  </si>
-  <si>
-    <t>Jun 2025</t>
   </si>
   <si>
     <t>Excess_Jan 2025</t>
@@ -396,9 +393,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -707,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -755,58 +755,58 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2">
+        <v>45809</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>141494.04999999999</v>
@@ -863,18 +863,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U2">
         <v>2</v>
       </c>
       <c r="V2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>220.02</v>
@@ -931,18 +931,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U3">
         <v>49</v>
       </c>
       <c r="V3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>50</v>
@@ -999,18 +999,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U4">
         <v>8</v>
       </c>
       <c r="V4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1067,18 +1067,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U5">
         <v>15</v>
       </c>
       <c r="V5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1135,18 +1135,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U6">
         <v>22</v>
       </c>
       <c r="V6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1203,18 +1203,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U7">
         <v>22</v>
       </c>
       <c r="V7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>11298.13</v>
@@ -1271,18 +1271,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U8">
         <v>75</v>
       </c>
       <c r="V8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>6112.59</v>
@@ -1339,18 +1339,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U9">
         <v>74</v>
       </c>
       <c r="V9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10">
         <v>6500.13</v>
@@ -1407,18 +1407,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U10">
         <v>31</v>
       </c>
       <c r="V10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11">
         <v>6653.87</v>
@@ -1475,18 +1475,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U11">
         <v>68</v>
       </c>
       <c r="V11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12">
         <v>2738.62</v>
@@ -1543,18 +1543,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U12">
         <v>61</v>
       </c>
       <c r="V12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13">
         <v>968</v>
@@ -1611,18 +1611,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U13">
         <v>50</v>
       </c>
       <c r="V13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>34271.339999999997</v>
@@ -1679,18 +1679,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U14">
         <v>78</v>
       </c>
       <c r="V14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1747,18 +1747,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U15">
         <v>22</v>
       </c>
       <c r="V15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>15541.84</v>
@@ -1815,18 +1815,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U16">
         <v>76</v>
       </c>
       <c r="V16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1883,18 +1883,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U17">
         <v>44</v>
       </c>
       <c r="V17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18">
         <v>15541.84</v>
@@ -1951,18 +1951,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U18">
         <v>77</v>
       </c>
       <c r="V18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19">
         <v>16000</v>
@@ -2019,18 +2019,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U19">
         <v>13</v>
       </c>
       <c r="V19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20">
         <v>123.45</v>
@@ -2087,18 +2087,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U20">
         <v>17</v>
       </c>
       <c r="V20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21">
         <v>737</v>
@@ -2155,18 +2155,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U21">
         <v>16</v>
       </c>
       <c r="V21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22">
         <v>860.45</v>
@@ -2223,18 +2223,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U22">
         <v>14</v>
       </c>
       <c r="V22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23">
         <v>711.34</v>
@@ -2291,18 +2291,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U23">
         <v>46</v>
       </c>
       <c r="V23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24">
         <v>204.97</v>
@@ -2359,18 +2359,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U24">
         <v>20</v>
       </c>
       <c r="V24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25">
         <v>2937.12</v>
@@ -2427,18 +2427,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U25">
         <v>7</v>
       </c>
       <c r="V25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26">
         <v>967.37</v>
@@ -2495,18 +2495,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U26">
         <v>57</v>
       </c>
       <c r="V26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27">
         <v>940.88</v>
@@ -2563,18 +2563,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U27">
         <v>56</v>
       </c>
       <c r="V27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28">
         <v>4545.8599999999997</v>
@@ -2631,18 +2631,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U28">
         <v>52</v>
       </c>
       <c r="V28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B29">
         <v>1250.69</v>
@@ -2699,18 +2699,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U29">
         <v>51</v>
       </c>
       <c r="V29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30">
         <v>6737.43</v>
@@ -2767,18 +2767,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U30">
         <v>62</v>
       </c>
       <c r="V30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -2835,18 +2835,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U31">
         <v>18</v>
       </c>
       <c r="V31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -2903,18 +2903,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U32">
         <v>10</v>
       </c>
       <c r="V32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33">
         <v>539.88</v>
@@ -2971,18 +2971,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U33">
         <v>32</v>
       </c>
       <c r="V33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -3039,18 +3039,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U34">
         <v>22</v>
       </c>
       <c r="V34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35">
         <v>5307.36</v>
@@ -3107,18 +3107,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U35">
         <v>12</v>
       </c>
       <c r="V35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B36">
         <v>264.38</v>
@@ -3175,18 +3175,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U36">
         <v>9</v>
       </c>
       <c r="V36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -3243,18 +3243,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U37">
         <v>6</v>
       </c>
       <c r="V37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B38">
         <v>5571.74</v>
@@ -3311,18 +3311,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U38">
         <v>5</v>
       </c>
       <c r="V38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -3379,18 +3379,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U39">
         <v>22</v>
       </c>
       <c r="V39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40">
         <v>76.099999999999994</v>
@@ -3447,18 +3447,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U40">
         <v>34</v>
       </c>
       <c r="V40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41">
         <v>157.29</v>
@@ -3515,18 +3515,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U41">
         <v>21</v>
       </c>
       <c r="V41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42">
         <v>233.39</v>
@@ -3583,18 +3583,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U42">
         <v>33</v>
       </c>
       <c r="V42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43">
         <v>5998.14</v>
@@ -3651,18 +3651,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U43">
         <v>69</v>
       </c>
       <c r="V43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44">
         <v>579.63</v>
@@ -3719,18 +3719,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U44">
         <v>54</v>
       </c>
       <c r="V44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B45">
         <v>3691.42</v>
@@ -3787,18 +3787,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U45">
         <v>55</v>
       </c>
       <c r="V45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B46">
         <v>10269.19</v>
@@ -3855,18 +3855,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U46">
         <v>73</v>
       </c>
       <c r="V46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B47">
         <v>396.58</v>
@@ -3923,18 +3923,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U47">
         <v>43</v>
       </c>
       <c r="V47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -3991,18 +3991,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U48">
         <v>22</v>
       </c>
       <c r="V48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B49">
         <v>1488.66</v>
@@ -4059,18 +4059,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U49">
         <v>58</v>
       </c>
       <c r="V49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B50">
         <v>578.99</v>
@@ -4127,18 +4127,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U50">
         <v>63</v>
       </c>
       <c r="V50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51">
         <v>2067.65</v>
@@ -4195,18 +4195,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U51">
         <v>66</v>
       </c>
       <c r="V51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B52">
         <v>799</v>
@@ -4263,18 +4263,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U52">
         <v>47</v>
       </c>
       <c r="V52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B53">
         <v>325.63</v>
@@ -4331,18 +4331,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U53">
         <v>48</v>
       </c>
       <c r="V53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -4399,18 +4399,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U54">
         <v>36</v>
       </c>
       <c r="V54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -4467,18 +4467,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U55">
         <v>19</v>
       </c>
       <c r="V55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -4535,18 +4535,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U56">
         <v>35</v>
       </c>
       <c r="V56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B57">
         <v>1333.34</v>
@@ -4603,18 +4603,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U57">
         <v>60</v>
       </c>
       <c r="V57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -4671,18 +4671,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U58">
         <v>42</v>
       </c>
       <c r="V58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -4739,18 +4739,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T59" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U59">
         <v>3</v>
       </c>
       <c r="V59" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -4807,18 +4807,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U60">
         <v>4</v>
       </c>
       <c r="V60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B61">
         <v>2648.43</v>
@@ -4875,18 +4875,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T61" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U61">
         <v>59</v>
       </c>
       <c r="V61" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B62">
         <v>380.77</v>
@@ -4943,18 +4943,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U62">
         <v>40</v>
       </c>
       <c r="V62" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B63">
         <v>172</v>
@@ -5011,18 +5011,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T63" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U63">
         <v>39</v>
       </c>
       <c r="V63" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B64">
         <v>700</v>
@@ -5079,18 +5079,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U64">
         <v>11</v>
       </c>
       <c r="V64" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -5147,18 +5147,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T65" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U65">
         <v>22</v>
       </c>
       <c r="V65" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B66">
         <v>100</v>
@@ -5215,18 +5215,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T66" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U66">
         <v>37</v>
       </c>
       <c r="V66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B67">
         <v>6967.81</v>
@@ -5283,18 +5283,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T67" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U67">
         <v>64</v>
       </c>
       <c r="V67" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -5351,18 +5351,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T68" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U68">
         <v>41</v>
       </c>
       <c r="V68" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B69">
         <v>7067.81</v>
@@ -5419,18 +5419,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U69">
         <v>65</v>
       </c>
       <c r="V69" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B70">
         <v>125</v>
@@ -5487,18 +5487,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T70" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U70">
         <v>38</v>
       </c>
       <c r="V70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B71">
         <v>14421.21</v>
@@ -5555,18 +5555,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T71" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U71">
         <v>71</v>
       </c>
       <c r="V71" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B72">
         <v>14546.21</v>
@@ -5623,18 +5623,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T72" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U72">
         <v>72</v>
       </c>
       <c r="V72" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -5691,18 +5691,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T73" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U73">
         <v>22</v>
       </c>
       <c r="V73" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B74">
         <v>604.98</v>
@@ -5759,18 +5759,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T74" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U74">
         <v>53</v>
       </c>
       <c r="V74" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B75">
         <v>211.54</v>
@@ -5827,18 +5827,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T75" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U75">
         <v>45</v>
       </c>
       <c r="V75" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B76">
         <v>3193.66</v>
@@ -5895,18 +5895,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T76" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U76">
         <v>67</v>
       </c>
       <c r="V76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B77">
         <v>4010.18</v>
@@ -5963,18 +5963,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T77" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U77">
         <v>70</v>
       </c>
       <c r="V77" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -6031,18 +6031,18 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T78" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U78">
         <v>22</v>
       </c>
       <c r="V78" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B79">
         <v>12470.41</v>
@@ -6099,13 +6099,13 @@
         <v>-3327.4642857142871</v>
       </c>
       <c r="T79" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U79">
         <v>1</v>
       </c>
       <c r="V79" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>